<commit_message>
combined ratings fix temp
</commit_message>
<xml_diff>
--- a/AndroidRatings.xlsx
+++ b/AndroidRatings.xlsx
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:31</t>
+          <t>2023-06-26 19:33:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:31</t>
+          <t>2023-06-26 19:33:36</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -553,7 +553,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:31</t>
+          <t>2023-06-26 19:33:36</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:32</t>
+          <t>2023-06-26 19:33:36</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -602,28 +602,28 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>90301</v>
+        <v>90306</v>
       </c>
       <c r="E5" t="n">
-        <v>67920</v>
+        <v>67936</v>
       </c>
       <c r="F5" t="n">
-        <v>10890</v>
+        <v>10885</v>
       </c>
       <c r="G5" t="n">
-        <v>3980</v>
+        <v>3978</v>
       </c>
       <c r="H5" t="n">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="I5" t="n">
-        <v>5991</v>
+        <v>5988</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:32</t>
+          <t>2023-06-26 19:33:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>996374</v>
+        <v>996382</v>
       </c>
       <c r="E6" t="n">
-        <v>770104</v>
+        <v>770094</v>
       </c>
       <c r="F6" t="n">
-        <v>153182</v>
+        <v>153163</v>
       </c>
       <c r="G6" t="n">
-        <v>29856</v>
+        <v>29864</v>
       </c>
       <c r="H6" t="n">
-        <v>7375</v>
+        <v>7386</v>
       </c>
       <c r="I6" t="n">
-        <v>35857</v>
+        <v>35875</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:32</t>
+          <t>2023-06-26 19:33:37</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -672,28 +672,28 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>190320</v>
+        <v>190322</v>
       </c>
       <c r="E7" t="n">
-        <v>128792</v>
+        <v>128793</v>
       </c>
       <c r="F7" t="n">
-        <v>18878</v>
+        <v>18885</v>
       </c>
       <c r="G7" t="n">
-        <v>8677</v>
+        <v>8676</v>
       </c>
       <c r="H7" t="n">
-        <v>6062</v>
+        <v>6061</v>
       </c>
       <c r="I7" t="n">
-        <v>27911</v>
+        <v>27907</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:32</t>
+          <t>2023-06-26 19:33:37</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -707,28 +707,28 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>59626</v>
+        <v>59628</v>
       </c>
       <c r="E8" t="n">
         <v>33889</v>
       </c>
       <c r="F8" t="n">
-        <v>4685</v>
+        <v>4683</v>
       </c>
       <c r="G8" t="n">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="H8" t="n">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="I8" t="n">
-        <v>15762</v>
+        <v>15768</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:33</t>
+          <t>2023-06-26 19:33:37</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -742,28 +742,28 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>774578</v>
+        <v>774579</v>
       </c>
       <c r="E9" t="n">
-        <v>426301</v>
+        <v>426307</v>
       </c>
       <c r="F9" t="n">
-        <v>71239</v>
+        <v>71238</v>
       </c>
       <c r="G9" t="n">
-        <v>42262</v>
+        <v>42261</v>
       </c>
       <c r="H9" t="n">
         <v>31181</v>
       </c>
       <c r="I9" t="n">
-        <v>203595</v>
+        <v>203592</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:33</t>
+          <t>2023-06-26 19:33:38</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,28 +777,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>12600</v>
+        <v>12599</v>
       </c>
       <c r="E10" t="n">
-        <v>5552</v>
+        <v>5558</v>
       </c>
       <c r="F10" t="n">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="G10" t="n">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H10" t="n">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I10" t="n">
-        <v>4452</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:33</t>
+          <t>2023-06-26 19:33:38</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -833,7 +833,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:33</t>
+          <t>2023-06-26 19:33:38</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -847,28 +847,28 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>635823</v>
+        <v>635843</v>
       </c>
       <c r="E12" t="n">
-        <v>481414</v>
+        <v>481462</v>
       </c>
       <c r="F12" t="n">
-        <v>106619</v>
+        <v>106587</v>
       </c>
       <c r="G12" t="n">
-        <v>29959</v>
+        <v>29969</v>
       </c>
       <c r="H12" t="n">
-        <v>4891</v>
+        <v>4890</v>
       </c>
       <c r="I12" t="n">
-        <v>12940</v>
+        <v>12935</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:34</t>
+          <t>2023-06-26 19:33:39</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -885,25 +885,25 @@
         <v>143482</v>
       </c>
       <c r="E13" t="n">
-        <v>92955</v>
+        <v>92959</v>
       </c>
       <c r="F13" t="n">
-        <v>19820</v>
+        <v>19819</v>
       </c>
       <c r="G13" t="n">
-        <v>7843</v>
+        <v>7842</v>
       </c>
       <c r="H13" t="n">
-        <v>3941</v>
+        <v>3940</v>
       </c>
       <c r="I13" t="n">
-        <v>18923</v>
+        <v>18922</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:34</t>
+          <t>2023-06-26 19:33:39</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:34</t>
+          <t>2023-06-26 19:33:39</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -952,13 +952,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>55354</v>
+        <v>55353</v>
       </c>
       <c r="E15" t="n">
-        <v>34532</v>
+        <v>34531</v>
       </c>
       <c r="F15" t="n">
-        <v>7788</v>
+        <v>7787</v>
       </c>
       <c r="G15" t="n">
         <v>3068</v>
@@ -967,13 +967,13 @@
         <v>1689</v>
       </c>
       <c r="I15" t="n">
-        <v>8277</v>
+        <v>8278</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:35</t>
+          <t>2023-06-26 19:33:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -987,28 +987,28 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>29613</v>
+        <v>29614</v>
       </c>
       <c r="E16" t="n">
-        <v>19420</v>
+        <v>19414</v>
       </c>
       <c r="F16" t="n">
-        <v>4318</v>
+        <v>4317</v>
       </c>
       <c r="G16" t="n">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="H16" t="n">
         <v>942</v>
       </c>
       <c r="I16" t="n">
-        <v>3186</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:35</t>
+          <t>2023-06-26 19:33:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1043,7 +1043,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:35</t>
+          <t>2023-06-26 19:33:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1057,28 +1057,28 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>189221</v>
+        <v>189232</v>
       </c>
       <c r="E18" t="n">
-        <v>145871</v>
+        <v>145886</v>
       </c>
       <c r="F18" t="n">
-        <v>28306</v>
+        <v>28301</v>
       </c>
       <c r="G18" t="n">
-        <v>7661</v>
+        <v>7666</v>
       </c>
       <c r="H18" t="n">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="I18" t="n">
-        <v>5640</v>
+        <v>5637</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:36</t>
+          <t>2023-06-26 19:33:41</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1092,28 +1092,28 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>277507</v>
+        <v>277508</v>
       </c>
       <c r="E19" t="n">
-        <v>106061</v>
+        <v>106057</v>
       </c>
       <c r="F19" t="n">
-        <v>20891</v>
+        <v>20890</v>
       </c>
       <c r="G19" t="n">
-        <v>16269</v>
+        <v>16280</v>
       </c>
       <c r="H19" t="n">
-        <v>19025</v>
+        <v>19024</v>
       </c>
       <c r="I19" t="n">
-        <v>115261</v>
+        <v>115257</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:36</t>
+          <t>2023-06-26 19:33:41</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:36</t>
+          <t>2023-06-26 19:33:41</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1183,7 +1183,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:37</t>
+          <t>2023-06-26 19:33:41</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1197,28 +1197,28 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>379628</v>
+        <v>379630</v>
       </c>
       <c r="E22" t="n">
-        <v>247632</v>
+        <v>247619</v>
       </c>
       <c r="F22" t="n">
-        <v>35993</v>
+        <v>36002</v>
       </c>
       <c r="G22" t="n">
-        <v>20625</v>
+        <v>20635</v>
       </c>
       <c r="H22" t="n">
-        <v>12253</v>
+        <v>12252</v>
       </c>
       <c r="I22" t="n">
-        <v>63125</v>
+        <v>63122</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:37</t>
+          <t>2023-06-26 19:33:42</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1232,28 +1232,28 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>36335</v>
+        <v>36336</v>
       </c>
       <c r="E23" t="n">
-        <v>24110</v>
+        <v>24114</v>
       </c>
       <c r="F23" t="n">
-        <v>4726</v>
+        <v>4725</v>
       </c>
       <c r="G23" t="n">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="H23" t="n">
         <v>940</v>
       </c>
       <c r="I23" t="n">
-        <v>4607</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:38</t>
+          <t>2023-06-26 19:33:42</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1267,28 +1267,28 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>153495</v>
+        <v>153507</v>
       </c>
       <c r="E24" t="n">
-        <v>80727</v>
+        <v>80750</v>
       </c>
       <c r="F24" t="n">
-        <v>15493</v>
+        <v>15514</v>
       </c>
       <c r="G24" t="n">
-        <v>9196</v>
+        <v>9181</v>
       </c>
       <c r="H24" t="n">
-        <v>7716</v>
+        <v>7712</v>
       </c>
       <c r="I24" t="n">
-        <v>40363</v>
+        <v>40350</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:38</t>
+          <t>2023-06-26 19:33:42</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1323,7 +1323,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:38</t>
+          <t>2023-06-26 19:33:43</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:39</t>
+          <t>2023-06-26 19:33:43</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1393,7 +1393,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:39</t>
+          <t>2023-06-26 19:33:43</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1414,7 +1414,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:39</t>
+          <t>2023-06-26 19:33:43</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1449,7 +1449,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:39</t>
+          <t>2023-06-26 19:33:44</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:40</t>
+          <t>2023-06-26 19:33:44</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1519,7 +1519,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:40</t>
+          <t>2023-06-26 19:33:44</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1554,7 +1554,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:40</t>
+          <t>2023-06-26 19:33:45</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1589,7 +1589,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:40</t>
+          <t>2023-06-26 19:33:45</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:41</t>
+          <t>2023-06-26 19:33:45</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2454</v>
+        <v>2455</v>
       </c>
       <c r="E35" t="n">
         <v>1304</v>
@@ -1653,13 +1653,13 @@
         <v>119</v>
       </c>
       <c r="I35" t="n">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:41</t>
+          <t>2023-06-26 19:33:45</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1694,7 +1694,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:41</t>
+          <t>2023-06-26 19:33:46</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1729,7 +1729,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-06-26 18:41:42</t>
+          <t>2023-06-26 19:33:46</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">

</xml_diff>

<commit_message>
Combined DF Update with Dashboard Tab 1
</commit_message>
<xml_diff>
--- a/AndroidRatings.xlsx
+++ b/AndroidRatings.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Date_A</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -483,497 +483,497 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:36</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Go Kinetic by Windstream</t>
+          <t>My altafiber</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>21044</v>
+        <v>317</v>
       </c>
       <c r="E2" t="n">
-        <v>15631</v>
+        <v>225</v>
       </c>
       <c r="F2" t="n">
-        <v>3227</v>
+        <v>43</v>
       </c>
       <c r="G2" t="n">
-        <v>689</v>
+        <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>149</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
-        <v>1348</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:36</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>My altafiber</t>
+          <t>myCricket</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>317</v>
+        <v>190325</v>
       </c>
       <c r="E3" t="n">
-        <v>225</v>
+        <v>128799</v>
       </c>
       <c r="F3" t="n">
-        <v>43</v>
+        <v>18881</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>8674</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>6060</v>
       </c>
       <c r="I3" t="n">
-        <v>33</v>
+        <v>27911</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:36</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Spectrum Access: Enabled Media</t>
+          <t>T-Mobile</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>142</v>
+        <v>774577</v>
       </c>
       <c r="E4" t="n">
-        <v>102</v>
+        <v>426306</v>
       </c>
       <c r="F4" t="n">
-        <v>21</v>
+        <v>71237</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>42262</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>31181</v>
       </c>
       <c r="I4" t="n">
-        <v>7</v>
+        <v>203591</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:36</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cox</t>
+          <t>MyDISH</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>90306</v>
+        <v>59628</v>
       </c>
       <c r="E5" t="n">
-        <v>67936</v>
+        <v>33889</v>
       </c>
       <c r="F5" t="n">
-        <v>10885</v>
+        <v>4683</v>
       </c>
       <c r="G5" t="n">
-        <v>3978</v>
+        <v>2482</v>
       </c>
       <c r="H5" t="n">
-        <v>1519</v>
+        <v>2806</v>
       </c>
       <c r="I5" t="n">
-        <v>5988</v>
+        <v>15768</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:37</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>My Verizon</t>
+          <t>My Sprint</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>996382</v>
+        <v>143484</v>
       </c>
       <c r="E6" t="n">
-        <v>770094</v>
+        <v>92953</v>
       </c>
       <c r="F6" t="n">
-        <v>153163</v>
+        <v>19818</v>
       </c>
       <c r="G6" t="n">
-        <v>29864</v>
+        <v>7842</v>
       </c>
       <c r="H6" t="n">
-        <v>7386</v>
+        <v>3941</v>
       </c>
       <c r="I6" t="n">
-        <v>35875</v>
+        <v>18930</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:37</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>myCricket</t>
+          <t>Verizon My Fios</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>190322</v>
+        <v>76745</v>
       </c>
       <c r="E7" t="n">
-        <v>128793</v>
+        <v>54744</v>
       </c>
       <c r="F7" t="n">
-        <v>18885</v>
+        <v>9188</v>
       </c>
       <c r="G7" t="n">
-        <v>8676</v>
+        <v>3687</v>
       </c>
       <c r="H7" t="n">
-        <v>6061</v>
+        <v>1762</v>
       </c>
       <c r="I7" t="n">
-        <v>27907</v>
+        <v>7364</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:37</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MyDISH</t>
+          <t>My Verizon</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>59628</v>
+        <v>996393</v>
       </c>
       <c r="E8" t="n">
-        <v>33889</v>
+        <v>770113</v>
       </c>
       <c r="F8" t="n">
-        <v>4683</v>
+        <v>153142</v>
       </c>
       <c r="G8" t="n">
-        <v>2482</v>
+        <v>29860</v>
       </c>
       <c r="H8" t="n">
-        <v>2806</v>
+        <v>7385</v>
       </c>
       <c r="I8" t="n">
-        <v>15768</v>
+        <v>35893</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:37</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>T-Mobile</t>
+          <t>Spectrum Access: Enabled Media</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>774579</v>
+        <v>142</v>
       </c>
       <c r="E9" t="n">
-        <v>426307</v>
+        <v>102</v>
       </c>
       <c r="F9" t="n">
-        <v>71238</v>
+        <v>21</v>
       </c>
       <c r="G9" t="n">
-        <v>42261</v>
+        <v>10</v>
       </c>
       <c r="H9" t="n">
-        <v>31181</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>203592</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:38</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Xfinity Mobile</t>
+          <t>My CenturyLink</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>12599</v>
+        <v>55353</v>
       </c>
       <c r="E10" t="n">
-        <v>5558</v>
+        <v>34532</v>
       </c>
       <c r="F10" t="n">
-        <v>895</v>
+        <v>7787</v>
       </c>
       <c r="G10" t="n">
-        <v>844</v>
+        <v>3068</v>
       </c>
       <c r="H10" t="n">
-        <v>854</v>
+        <v>1689</v>
       </c>
       <c r="I10" t="n">
-        <v>4448</v>
+        <v>8277</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:38</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Spectrum News: Local Stories</t>
+          <t>Xfinity Mobile</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5393</v>
+        <v>12601</v>
       </c>
       <c r="E11" t="n">
-        <v>3239</v>
+        <v>5559</v>
       </c>
       <c r="F11" t="n">
-        <v>782</v>
+        <v>895</v>
       </c>
       <c r="G11" t="n">
-        <v>410</v>
+        <v>844</v>
       </c>
       <c r="H11" t="n">
-        <v>270</v>
+        <v>854</v>
       </c>
       <c r="I11" t="n">
-        <v>692</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:38</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>My Spectrum</t>
+          <t>Spectrum News: Local Stories</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>635843</v>
+        <v>5393</v>
       </c>
       <c r="E12" t="n">
-        <v>481462</v>
+        <v>3239</v>
       </c>
       <c r="F12" t="n">
-        <v>106587</v>
+        <v>782</v>
       </c>
       <c r="G12" t="n">
-        <v>29969</v>
+        <v>410</v>
       </c>
       <c r="H12" t="n">
-        <v>4890</v>
+        <v>270</v>
       </c>
       <c r="I12" t="n">
-        <v>12935</v>
+        <v>692</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:39</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>My Sprint</t>
+          <t>Cox</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>143482</v>
+        <v>90307</v>
       </c>
       <c r="E13" t="n">
-        <v>92959</v>
+        <v>67948</v>
       </c>
       <c r="F13" t="n">
-        <v>19819</v>
+        <v>10880</v>
       </c>
       <c r="G13" t="n">
-        <v>7842</v>
+        <v>3976</v>
       </c>
       <c r="H13" t="n">
-        <v>3940</v>
+        <v>1518</v>
       </c>
       <c r="I13" t="n">
-        <v>18922</v>
+        <v>5985</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:39</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Verizon My Fios</t>
+          <t>My Spectrum</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>76741</v>
+        <v>635870</v>
       </c>
       <c r="E14" t="n">
-        <v>54739</v>
+        <v>481448</v>
       </c>
       <c r="F14" t="n">
-        <v>9192</v>
+        <v>106596</v>
       </c>
       <c r="G14" t="n">
-        <v>3689</v>
+        <v>29988</v>
       </c>
       <c r="H14" t="n">
-        <v>1763</v>
+        <v>4888</v>
       </c>
       <c r="I14" t="n">
-        <v>7358</v>
+        <v>12950</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:39</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>My CenturyLink</t>
+          <t>Go Kinetic by Windstream</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>55353</v>
+        <v>21046</v>
       </c>
       <c r="E15" t="n">
-        <v>34531</v>
+        <v>15637</v>
       </c>
       <c r="F15" t="n">
-        <v>7787</v>
+        <v>3225</v>
       </c>
       <c r="G15" t="n">
-        <v>3068</v>
+        <v>688</v>
       </c>
       <c r="H15" t="n">
-        <v>1689</v>
+        <v>149</v>
       </c>
       <c r="I15" t="n">
-        <v>8278</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:40</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -987,10 +987,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>29614</v>
+        <v>29613</v>
       </c>
       <c r="E16" t="n">
-        <v>19414</v>
+        <v>19413</v>
       </c>
       <c r="F16" t="n">
         <v>4317</v>
@@ -1008,7 +1008,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:40</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1043,147 +1043,133 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:40</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Spectrum TV</t>
+          <t>Spectrum SportsNet: Live Games</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>189232</v>
+        <v>1416</v>
       </c>
       <c r="E18" t="n">
-        <v>145886</v>
+        <v>635</v>
       </c>
       <c r="F18" t="n">
-        <v>28301</v>
+        <v>158</v>
       </c>
       <c r="G18" t="n">
-        <v>7666</v>
+        <v>63</v>
       </c>
       <c r="H18" t="n">
-        <v>1742</v>
+        <v>52</v>
       </c>
       <c r="I18" t="n">
-        <v>5637</v>
+        <v>508</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:41</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>myAT&amp;T</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
+          <t>Astound Mobile</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>277508</v>
-      </c>
-      <c r="E19" t="n">
-        <v>106057</v>
-      </c>
-      <c r="F19" t="n">
-        <v>20890</v>
-      </c>
-      <c r="G19" t="n">
-        <v>16280</v>
-      </c>
-      <c r="H19" t="n">
-        <v>19024</v>
-      </c>
-      <c r="I19" t="n">
-        <v>115257</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:41</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Spectrum SportsNet: Live Games</t>
+          <t>Armstrong</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1416</v>
+        <v>459</v>
       </c>
       <c r="E20" t="n">
-        <v>635</v>
+        <v>286</v>
       </c>
       <c r="F20" t="n">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="G20" t="n">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="H20" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="I20" t="n">
-        <v>508</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:41</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MediacomConnect</t>
+          <t>Google Fiber</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>12518</v>
+        <v>1153</v>
       </c>
       <c r="E21" t="n">
-        <v>5974</v>
+        <v>690</v>
       </c>
       <c r="F21" t="n">
-        <v>1525</v>
+        <v>90</v>
       </c>
       <c r="G21" t="n">
-        <v>823</v>
+        <v>80</v>
       </c>
       <c r="H21" t="n">
-        <v>923</v>
+        <v>60</v>
       </c>
       <c r="I21" t="n">
-        <v>3273</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:41</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1197,28 +1183,28 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>379630</v>
+        <v>379632</v>
       </c>
       <c r="E22" t="n">
-        <v>247619</v>
+        <v>247636</v>
       </c>
       <c r="F22" t="n">
-        <v>36002</v>
+        <v>35998</v>
       </c>
       <c r="G22" t="n">
-        <v>20635</v>
+        <v>20633</v>
       </c>
       <c r="H22" t="n">
-        <v>12252</v>
+        <v>12250</v>
       </c>
       <c r="I22" t="n">
-        <v>63122</v>
+        <v>63115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:42</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1232,13 +1218,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>36336</v>
+        <v>36337</v>
       </c>
       <c r="E23" t="n">
-        <v>24114</v>
+        <v>24118</v>
       </c>
       <c r="F23" t="n">
-        <v>4725</v>
+        <v>4723</v>
       </c>
       <c r="G23" t="n">
         <v>1951</v>
@@ -1247,214 +1233,228 @@
         <v>940</v>
       </c>
       <c r="I23" t="n">
-        <v>4606</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:42</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Xfinity</t>
+          <t>HughesNet Mobile</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>153507</v>
+        <v>1538</v>
       </c>
       <c r="E24" t="n">
-        <v>80750</v>
+        <v>534</v>
       </c>
       <c r="F24" t="n">
-        <v>15514</v>
+        <v>98</v>
       </c>
       <c r="G24" t="n">
-        <v>9181</v>
+        <v>109</v>
       </c>
       <c r="H24" t="n">
-        <v>7712</v>
+        <v>87</v>
       </c>
       <c r="I24" t="n">
-        <v>40350</v>
+        <v>710</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:42</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Google Fiber</t>
+          <t>myAT&amp;T</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1153</v>
+        <v>277511</v>
       </c>
       <c r="E25" t="n">
-        <v>690</v>
+        <v>106068</v>
       </c>
       <c r="F25" t="n">
-        <v>90</v>
+        <v>20887</v>
       </c>
       <c r="G25" t="n">
-        <v>80</v>
+        <v>16278</v>
       </c>
       <c r="H25" t="n">
-        <v>60</v>
+        <v>19022</v>
       </c>
       <c r="I25" t="n">
-        <v>233</v>
+        <v>115256</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:43</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>My Viasat</t>
+          <t>MediacomConnect</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2954</v>
+        <v>12518</v>
       </c>
       <c r="E26" t="n">
-        <v>1448</v>
+        <v>5974</v>
       </c>
       <c r="F26" t="n">
-        <v>449</v>
+        <v>1525</v>
       </c>
       <c r="G26" t="n">
-        <v>229</v>
+        <v>823</v>
       </c>
       <c r="H26" t="n">
-        <v>69</v>
+        <v>923</v>
       </c>
       <c r="I26" t="n">
-        <v>759</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:43</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Armstrong</t>
+          <t>Spectrum TV</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>459</v>
+        <v>189244</v>
       </c>
       <c r="E27" t="n">
-        <v>286</v>
+        <v>145902</v>
       </c>
       <c r="F27" t="n">
-        <v>73</v>
+        <v>28305</v>
       </c>
       <c r="G27" t="n">
-        <v>27</v>
+        <v>7662</v>
       </c>
       <c r="H27" t="n">
-        <v>13</v>
+        <v>1741</v>
       </c>
       <c r="I27" t="n">
-        <v>60</v>
+        <v>5634</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:43</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Astound Mobile</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
+          <t>My Viasat</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
       <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+        <v>2954</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1448</v>
+      </c>
+      <c r="F28" t="n">
+        <v>449</v>
+      </c>
+      <c r="G28" t="n">
+        <v>229</v>
+      </c>
+      <c r="H28" t="n">
+        <v>69</v>
+      </c>
+      <c r="I28" t="n">
+        <v>759</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:43</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>HughesNet Mobile</t>
+          <t>Xfinity</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1538</v>
+        <v>153512</v>
       </c>
       <c r="E29" t="n">
-        <v>535</v>
+        <v>80746</v>
       </c>
       <c r="F29" t="n">
-        <v>98</v>
+        <v>15515</v>
       </c>
       <c r="G29" t="n">
-        <v>109</v>
+        <v>9176</v>
       </c>
       <c r="H29" t="n">
-        <v>87</v>
+        <v>7717</v>
       </c>
       <c r="I29" t="n">
-        <v>709</v>
+        <v>40358</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:44</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>HT My Account</t>
+          <t>Optimum Support</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1463,98 +1463,98 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>33</v>
+        <v>1226</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>386</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G30" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="H30" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="I30" t="n">
-        <v>18</v>
+        <v>703</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:44</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Midco My Account</t>
+          <t>HT My Account</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>263</v>
+        <v>33</v>
       </c>
       <c r="E31" t="n">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="H31" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I31" t="n">
-        <v>151</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:44</t>
+          <t>2023-06-26 21:05:43</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Optimum Support</t>
+          <t>Midco My Account</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1226</v>
+        <v>263</v>
       </c>
       <c r="E32" t="n">
-        <v>386</v>
+        <v>74</v>
       </c>
       <c r="F32" t="n">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="H32" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I32" t="n">
-        <v>703</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:45</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1568,10 +1568,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>20519</v>
+        <v>20520</v>
       </c>
       <c r="E33" t="n">
-        <v>12673</v>
+        <v>12674</v>
       </c>
       <c r="F33" t="n">
         <v>2956</v>
@@ -1589,7 +1589,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:45</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1624,77 +1624,77 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:45</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Optimum TV</t>
+          <t>myBuckeye</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2455</v>
+        <v>79</v>
       </c>
       <c r="E35" t="n">
-        <v>1304</v>
+        <v>32</v>
       </c>
       <c r="F35" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="G35" t="n">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="H35" t="n">
-        <v>119</v>
+        <v>4</v>
       </c>
       <c r="I35" t="n">
-        <v>562</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:45</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Breezeline TV</t>
+          <t>Optimum TV</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>174</v>
+        <v>2457</v>
       </c>
       <c r="E36" t="n">
-        <v>38</v>
+        <v>1300</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="G36" t="n">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="H36" t="n">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="I36" t="n">
-        <v>121</v>
+        <v>570</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:46</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1708,10 +1708,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="E37" t="n">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F37" t="n">
         <v>88</v>
@@ -1720,7 +1720,7 @@
         <v>26</v>
       </c>
       <c r="H37" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I37" t="n">
         <v>61</v>
@@ -1729,36 +1729,36 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-06-26 19:33:46</t>
+          <t>2023-06-26 21:05:44</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>myBuckeye</t>
+          <t>Breezeline TV</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="E38" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F38" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H38" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I38" t="n">
-        <v>31</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
App Index Values for Dataframe Join
</commit_message>
<xml_diff>
--- a/AndroidRatings.xlsx
+++ b/AndroidRatings.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date_A</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -456,37 +456,39 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Android 5 Star Reviews</t>
+          <t>5 Star Reviews</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Android 4 Star Reviews</t>
+          <t>4 Star Reviews</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Android 3 Star Reviews</t>
+          <t>3 Star Reviews</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Android 2 Star Reviews</t>
+          <t>2 Star Reviews</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Android 1 Star Reviews</t>
+          <t>1 Star Reviews</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>GKW</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -500,31 +502,33 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>21046</v>
+        <v>21051</v>
       </c>
       <c r="F2" t="n">
         <v>15637</v>
       </c>
       <c r="G2" t="n">
-        <v>3225</v>
+        <v>3221</v>
       </c>
       <c r="H2" t="n">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="I2" t="n">
         <v>149</v>
       </c>
       <c r="J2" t="n">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>MAF</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,35 +538,37 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F3" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G3" t="n">
         <v>43</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>SAEM</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -595,12 +601,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -614,31 +622,33 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>90313</v>
+        <v>90346</v>
       </c>
       <c r="F5" t="n">
-        <v>67959</v>
+        <v>67999</v>
       </c>
       <c r="G5" t="n">
-        <v>10877</v>
+        <v>10921</v>
       </c>
       <c r="H5" t="n">
-        <v>3975</v>
+        <v>3961</v>
       </c>
       <c r="I5" t="n">
-        <v>1518</v>
+        <v>1512</v>
       </c>
       <c r="J5" t="n">
-        <v>5984</v>
+        <v>5953</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>MV</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -652,31 +662,33 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>996398</v>
+        <v>996577</v>
       </c>
       <c r="F6" t="n">
-        <v>770126</v>
+        <v>770332</v>
       </c>
       <c r="G6" t="n">
-        <v>153136</v>
+        <v>153103</v>
       </c>
       <c r="H6" t="n">
-        <v>29859</v>
+        <v>29849</v>
       </c>
       <c r="I6" t="n">
-        <v>7385</v>
+        <v>7402</v>
       </c>
       <c r="J6" t="n">
-        <v>35892</v>
+        <v>35891</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>MC</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -690,31 +702,33 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>190328</v>
+        <v>190361</v>
       </c>
       <c r="F7" t="n">
-        <v>128803</v>
+        <v>128814</v>
       </c>
       <c r="G7" t="n">
-        <v>18880</v>
+        <v>18867</v>
       </c>
       <c r="H7" t="n">
-        <v>8674</v>
+        <v>8659</v>
       </c>
       <c r="I7" t="n">
-        <v>6060</v>
+        <v>6069</v>
       </c>
       <c r="J7" t="n">
-        <v>27911</v>
+        <v>27952</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -728,31 +742,33 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>59629</v>
+        <v>59636</v>
       </c>
       <c r="F8" t="n">
-        <v>33894</v>
+        <v>33915</v>
       </c>
       <c r="G8" t="n">
-        <v>4682</v>
+        <v>4671</v>
       </c>
       <c r="H8" t="n">
-        <v>2482</v>
+        <v>2486</v>
       </c>
       <c r="I8" t="n">
-        <v>2805</v>
+        <v>2810</v>
       </c>
       <c r="J8" t="n">
-        <v>15766</v>
+        <v>15754</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>TM</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -766,31 +782,33 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>774577</v>
+        <v>774592</v>
       </c>
       <c r="F9" t="n">
-        <v>426306</v>
+        <v>426285</v>
       </c>
       <c r="G9" t="n">
-        <v>71237</v>
+        <v>71234</v>
       </c>
       <c r="H9" t="n">
-        <v>42262</v>
+        <v>42257</v>
       </c>
       <c r="I9" t="n">
-        <v>31181</v>
+        <v>31180</v>
       </c>
       <c r="J9" t="n">
-        <v>203591</v>
+        <v>203636</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>XM</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -804,31 +822,33 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>12601</v>
+        <v>12608</v>
       </c>
       <c r="F10" t="n">
-        <v>5559</v>
+        <v>5585</v>
       </c>
       <c r="G10" t="n">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="H10" t="n">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="I10" t="n">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="J10" t="n">
-        <v>4449</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>SNLS</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -842,13 +862,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>5393</v>
+        <v>5396</v>
       </c>
       <c r="F11" t="n">
-        <v>3239</v>
+        <v>3234</v>
       </c>
       <c r="G11" t="n">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="H11" t="n">
         <v>410</v>
@@ -857,16 +877,18 @@
         <v>270</v>
       </c>
       <c r="J11" t="n">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>MSA</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -880,31 +902,33 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>635887</v>
+        <v>636278</v>
       </c>
       <c r="F12" t="n">
-        <v>481446</v>
+        <v>481912</v>
       </c>
       <c r="G12" t="n">
-        <v>106604</v>
+        <v>106685</v>
       </c>
       <c r="H12" t="n">
-        <v>29992</v>
+        <v>29910</v>
       </c>
       <c r="I12" t="n">
-        <v>4897</v>
+        <v>4855</v>
       </c>
       <c r="J12" t="n">
-        <v>12948</v>
+        <v>12916</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>MSP</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -921,28 +945,30 @@
         <v>143482</v>
       </c>
       <c r="F13" t="n">
-        <v>92952</v>
+        <v>92945</v>
       </c>
       <c r="G13" t="n">
-        <v>19818</v>
+        <v>19817</v>
       </c>
       <c r="H13" t="n">
-        <v>7842</v>
+        <v>7841</v>
       </c>
       <c r="I13" t="n">
         <v>3940</v>
       </c>
       <c r="J13" t="n">
-        <v>18930</v>
+        <v>18939</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>VMF</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -956,31 +982,33 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>76745</v>
+        <v>76780</v>
       </c>
       <c r="F14" t="n">
-        <v>54747</v>
+        <v>54775</v>
       </c>
       <c r="G14" t="n">
-        <v>9187</v>
+        <v>9155</v>
       </c>
       <c r="H14" t="n">
-        <v>3686</v>
+        <v>3696</v>
       </c>
       <c r="I14" t="n">
-        <v>1762</v>
+        <v>1752</v>
       </c>
       <c r="J14" t="n">
-        <v>7363</v>
+        <v>7402</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MCL</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -994,31 +1022,33 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>55353</v>
+        <v>55363</v>
       </c>
       <c r="F15" t="n">
-        <v>34531</v>
+        <v>34509</v>
       </c>
       <c r="G15" t="n">
-        <v>7788</v>
+        <v>7783</v>
       </c>
       <c r="H15" t="n">
-        <v>3068</v>
+        <v>3073</v>
       </c>
       <c r="I15" t="n">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="J15" t="n">
-        <v>8277</v>
+        <v>8312</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>VM</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1032,31 +1062,33 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>29615</v>
+        <v>29627</v>
       </c>
       <c r="F16" t="n">
         <v>19421</v>
       </c>
       <c r="G16" t="n">
-        <v>4314</v>
+        <v>4315</v>
       </c>
       <c r="H16" t="n">
-        <v>1745</v>
+        <v>1737</v>
       </c>
       <c r="I16" t="n">
-        <v>942</v>
+        <v>948</v>
       </c>
       <c r="J16" t="n">
-        <v>3193</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>SU</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1089,12 +1121,14 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>STVA</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1108,31 +1142,33 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>189249</v>
+        <v>189314</v>
       </c>
       <c r="F18" t="n">
-        <v>145918</v>
+        <v>145954</v>
       </c>
       <c r="G18" t="n">
-        <v>28298</v>
+        <v>28269</v>
       </c>
       <c r="H18" t="n">
-        <v>7660</v>
+        <v>7704</v>
       </c>
       <c r="I18" t="n">
-        <v>1740</v>
+        <v>1734</v>
       </c>
       <c r="J18" t="n">
-        <v>5633</v>
+        <v>5653</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>ATT</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1146,31 +1182,33 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>277508</v>
+        <v>277534</v>
       </c>
       <c r="F19" t="n">
-        <v>106074</v>
+        <v>106095</v>
       </c>
       <c r="G19" t="n">
-        <v>20887</v>
+        <v>20836</v>
       </c>
       <c r="H19" t="n">
-        <v>16276</v>
+        <v>16261</v>
       </c>
       <c r="I19" t="n">
-        <v>19021</v>
+        <v>19011</v>
       </c>
       <c r="J19" t="n">
-        <v>115250</v>
+        <v>115331</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>SSLG</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1203,12 +1241,14 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>MDCM</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1225,28 +1265,30 @@
         <v>12518</v>
       </c>
       <c r="F21" t="n">
-        <v>5974</v>
+        <v>5980</v>
       </c>
       <c r="G21" t="n">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="H21" t="n">
         <v>823</v>
       </c>
       <c r="I21" t="n">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="J21" t="n">
-        <v>3273</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1260,31 +1302,33 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>379635</v>
+        <v>379646</v>
       </c>
       <c r="F22" t="n">
-        <v>247634</v>
+        <v>247755</v>
       </c>
       <c r="G22" t="n">
-        <v>35997</v>
+        <v>36015</v>
       </c>
       <c r="H22" t="n">
-        <v>20642</v>
+        <v>20490</v>
       </c>
       <c r="I22" t="n">
-        <v>12250</v>
+        <v>12270</v>
       </c>
       <c r="J22" t="n">
-        <v>63112</v>
+        <v>63116</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>MFR</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1298,31 +1342,33 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>36338</v>
+        <v>36356</v>
       </c>
       <c r="F23" t="n">
-        <v>24118</v>
+        <v>24053</v>
       </c>
       <c r="G23" t="n">
-        <v>4724</v>
+        <v>4748</v>
       </c>
       <c r="H23" t="n">
-        <v>1951</v>
+        <v>1988</v>
       </c>
       <c r="I23" t="n">
-        <v>940</v>
+        <v>969</v>
       </c>
       <c r="J23" t="n">
-        <v>4605</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>XF</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1336,31 +1382,33 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>153523</v>
+        <v>153663</v>
       </c>
       <c r="F24" t="n">
-        <v>80754</v>
+        <v>80655</v>
       </c>
       <c r="G24" t="n">
-        <v>15509</v>
+        <v>15428</v>
       </c>
       <c r="H24" t="n">
-        <v>9173</v>
+        <v>9174</v>
       </c>
       <c r="I24" t="n">
-        <v>7715</v>
+        <v>7713</v>
       </c>
       <c r="J24" t="n">
-        <v>40372</v>
+        <v>40693</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>GFBR</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1393,12 +1441,14 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>MVIA</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1412,31 +1462,33 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2954</v>
+        <v>2950</v>
       </c>
       <c r="F26" t="n">
         <v>1448</v>
       </c>
       <c r="G26" t="n">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H26" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I26" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J26" t="n">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>ARM</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1469,12 +1521,14 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>ASTRCN</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1493,12 +1547,14 @@
       <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>HUGH</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1512,10 +1568,10 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="F29" t="n">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="G29" t="n">
         <v>98</v>
@@ -1531,12 +1587,14 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>HTMYA</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1569,12 +1627,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>MIDCO</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1584,7 +1644,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1607,50 +1667,54 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>OPTS</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>June 27, 2023</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Optimum Support</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1227</v>
+      </c>
+      <c r="F32" t="n">
+        <v>382</v>
+      </c>
+      <c r="G32" t="n">
+        <v>70</v>
+      </c>
+      <c r="H32" t="n">
+        <v>50</v>
+      </c>
+      <c r="I32" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>June 26, 2023</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Optimum Support</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2.5</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>1226</v>
-      </c>
-      <c r="F32" t="n">
-        <v>386</v>
-      </c>
-      <c r="G32" t="n">
-        <v>69</v>
-      </c>
-      <c r="H32" t="n">
-        <v>39</v>
-      </c>
-      <c r="I32" t="n">
-        <v>29</v>
-      </c>
       <c r="J32" t="n">
-        <v>703</v>
+        <v>695</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>USCELL</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1664,31 +1728,33 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>20520</v>
+        <v>20526</v>
       </c>
       <c r="F33" t="n">
-        <v>12674</v>
+        <v>12685</v>
       </c>
       <c r="G33" t="n">
-        <v>2956</v>
+        <v>2947</v>
       </c>
       <c r="H33" t="n">
-        <v>1817</v>
+        <v>1821</v>
       </c>
       <c r="I33" t="n">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="J33" t="n">
-        <v>2455</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>SEC</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1721,12 +1787,14 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>OPTTV</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1736,35 +1804,37 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2456</v>
+        <v>2462</v>
       </c>
       <c r="F35" t="n">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="G35" t="n">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="H35" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I35" t="n">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="J35" t="n">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BRE</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1797,12 +1867,14 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>BLUER</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1816,31 +1888,33 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="F37" t="n">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G37" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H37" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I37" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J37" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>BUCK</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>June 26, 2023</t>
+          <t>June 27, 2023</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">

</xml_diff>

<commit_message>
iOS and Android Database Tables; Detail Date iOS
</commit_message>
<xml_diff>
--- a/AndroidRatings.xlsx
+++ b/AndroidRatings.xlsx
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>21053</v>
+        <v>21054</v>
       </c>
       <c r="F2" t="n">
-        <v>15644</v>
+        <v>15651</v>
       </c>
       <c r="G2" t="n">
-        <v>3218</v>
+        <v>3215</v>
       </c>
       <c r="H2" t="n">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I2" t="n">
         <v>149</v>
       </c>
       <c r="J2" t="n">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="3">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>90347</v>
+        <v>90356</v>
       </c>
       <c r="F5" t="n">
-        <v>68005</v>
+        <v>68024</v>
       </c>
       <c r="G5" t="n">
-        <v>10919</v>
+        <v>10918</v>
       </c>
       <c r="H5" t="n">
-        <v>3960</v>
+        <v>3957</v>
       </c>
       <c r="I5" t="n">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="J5" t="n">
-        <v>5951</v>
+        <v>5946</v>
       </c>
     </row>
     <row r="6">
@@ -662,22 +662,22 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>996589</v>
+        <v>996634</v>
       </c>
       <c r="F6" t="n">
-        <v>770364</v>
+        <v>770481</v>
       </c>
       <c r="G6" t="n">
-        <v>153082</v>
+        <v>152960</v>
       </c>
       <c r="H6" t="n">
-        <v>29845</v>
+        <v>29922</v>
       </c>
       <c r="I6" t="n">
-        <v>7401</v>
+        <v>7385</v>
       </c>
       <c r="J6" t="n">
-        <v>35897</v>
+        <v>35886</v>
       </c>
     </row>
     <row r="7">
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>190362</v>
+        <v>190369</v>
       </c>
       <c r="F7" t="n">
-        <v>128809</v>
+        <v>128924</v>
       </c>
       <c r="G7" t="n">
-        <v>18876</v>
+        <v>18822</v>
       </c>
       <c r="H7" t="n">
-        <v>8658</v>
+        <v>8638</v>
       </c>
       <c r="I7" t="n">
-        <v>6069</v>
+        <v>6087</v>
       </c>
       <c r="J7" t="n">
-        <v>27950</v>
+        <v>27898</v>
       </c>
     </row>
     <row r="8">
@@ -745,19 +745,19 @@
         <v>59636</v>
       </c>
       <c r="F8" t="n">
-        <v>33915</v>
+        <v>33924</v>
       </c>
       <c r="G8" t="n">
-        <v>4671</v>
+        <v>4669</v>
       </c>
       <c r="H8" t="n">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="I8" t="n">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="J8" t="n">
-        <v>15754</v>
+        <v>15749</v>
       </c>
     </row>
     <row r="9">
@@ -782,22 +782,22 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>774597</v>
+        <v>774599</v>
       </c>
       <c r="F9" t="n">
-        <v>426258</v>
+        <v>426262</v>
       </c>
       <c r="G9" t="n">
-        <v>71240</v>
+        <v>71245</v>
       </c>
       <c r="H9" t="n">
-        <v>42266</v>
+        <v>42263</v>
       </c>
       <c r="I9" t="n">
-        <v>31178</v>
+        <v>31177</v>
       </c>
       <c r="J9" t="n">
-        <v>203655</v>
+        <v>203652</v>
       </c>
     </row>
     <row r="10">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>12608</v>
+        <v>12607</v>
       </c>
       <c r="F10" t="n">
-        <v>5585</v>
+        <v>5572</v>
       </c>
       <c r="G10" t="n">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="H10" t="n">
-        <v>847</v>
+        <v>865</v>
       </c>
       <c r="I10" t="n">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="J10" t="n">
-        <v>4421</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="11">
@@ -902,22 +902,22 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>636310</v>
+        <v>636398</v>
       </c>
       <c r="F12" t="n">
-        <v>481931</v>
+        <v>482049</v>
       </c>
       <c r="G12" t="n">
-        <v>106709</v>
+        <v>106661</v>
       </c>
       <c r="H12" t="n">
-        <v>29897</v>
+        <v>29918</v>
       </c>
       <c r="I12" t="n">
-        <v>4852</v>
+        <v>4846</v>
       </c>
       <c r="J12" t="n">
-        <v>12921</v>
+        <v>12924</v>
       </c>
     </row>
     <row r="13">
@@ -942,13 +942,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>143482</v>
+        <v>143481</v>
       </c>
       <c r="F13" t="n">
         <v>92945</v>
       </c>
       <c r="G13" t="n">
-        <v>19817</v>
+        <v>19816</v>
       </c>
       <c r="H13" t="n">
         <v>7841</v>
@@ -982,22 +982,22 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>76783</v>
+        <v>76782</v>
       </c>
       <c r="F14" t="n">
-        <v>54783</v>
+        <v>54769</v>
       </c>
       <c r="G14" t="n">
-        <v>9153</v>
+        <v>9150</v>
       </c>
       <c r="H14" t="n">
-        <v>3695</v>
+        <v>3704</v>
       </c>
       <c r="I14" t="n">
         <v>1751</v>
       </c>
       <c r="J14" t="n">
-        <v>7401</v>
+        <v>7408</v>
       </c>
     </row>
     <row r="15">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>55366</v>
+        <v>55369</v>
       </c>
       <c r="F15" t="n">
-        <v>34514</v>
+        <v>34520</v>
       </c>
       <c r="G15" t="n">
-        <v>7782</v>
+        <v>7774</v>
       </c>
       <c r="H15" t="n">
-        <v>3073</v>
+        <v>3069</v>
       </c>
       <c r="I15" t="n">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="J15" t="n">
-        <v>8311</v>
+        <v>8322</v>
       </c>
     </row>
     <row r="16">
@@ -1062,22 +1062,22 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>29627</v>
+        <v>29631</v>
       </c>
       <c r="F16" t="n">
-        <v>19424</v>
+        <v>19413</v>
       </c>
       <c r="G16" t="n">
-        <v>4313</v>
+        <v>4311</v>
       </c>
       <c r="H16" t="n">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="I16" t="n">
         <v>948</v>
       </c>
       <c r="J16" t="n">
-        <v>3205</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="17">
@@ -1142,22 +1142,22 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>189322</v>
+        <v>189351</v>
       </c>
       <c r="F18" t="n">
-        <v>145968</v>
+        <v>145953</v>
       </c>
       <c r="G18" t="n">
-        <v>28258</v>
+        <v>28312</v>
       </c>
       <c r="H18" t="n">
-        <v>7701</v>
+        <v>7691</v>
       </c>
       <c r="I18" t="n">
-        <v>1744</v>
+        <v>1752</v>
       </c>
       <c r="J18" t="n">
-        <v>5651</v>
+        <v>5643</v>
       </c>
     </row>
     <row r="19">
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>277541</v>
+        <v>277543</v>
       </c>
       <c r="F19" t="n">
-        <v>106088</v>
+        <v>106098</v>
       </c>
       <c r="G19" t="n">
-        <v>20843</v>
+        <v>20840</v>
       </c>
       <c r="H19" t="n">
-        <v>16259</v>
+        <v>16268</v>
       </c>
       <c r="I19" t="n">
-        <v>19007</v>
+        <v>18994</v>
       </c>
       <c r="J19" t="n">
-        <v>115344</v>
+        <v>115343</v>
       </c>
     </row>
     <row r="20">
@@ -1262,19 +1262,19 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>12519</v>
+        <v>12520</v>
       </c>
       <c r="F21" t="n">
-        <v>5979</v>
+        <v>5980</v>
       </c>
       <c r="G21" t="n">
-        <v>1527</v>
+        <v>1517</v>
       </c>
       <c r="H21" t="n">
         <v>823</v>
       </c>
       <c r="I21" t="n">
-        <v>924</v>
+        <v>934</v>
       </c>
       <c r="J21" t="n">
         <v>3266</v>
@@ -1302,22 +1302,22 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>379651</v>
+        <v>379657</v>
       </c>
       <c r="F22" t="n">
-        <v>247762</v>
+        <v>247760</v>
       </c>
       <c r="G22" t="n">
-        <v>36022</v>
+        <v>36036</v>
       </c>
       <c r="H22" t="n">
-        <v>20489</v>
+        <v>20495</v>
       </c>
       <c r="I22" t="n">
-        <v>12268</v>
+        <v>12266</v>
       </c>
       <c r="J22" t="n">
-        <v>63110</v>
+        <v>63100</v>
       </c>
     </row>
     <row r="23">
@@ -1342,22 +1342,22 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>36357</v>
+        <v>36362</v>
       </c>
       <c r="F23" t="n">
-        <v>24057</v>
+        <v>24051</v>
       </c>
       <c r="G23" t="n">
-        <v>4747</v>
+        <v>4749</v>
       </c>
       <c r="H23" t="n">
-        <v>1988</v>
+        <v>1995</v>
       </c>
       <c r="I23" t="n">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="J23" t="n">
-        <v>4597</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="24">
@@ -1382,22 +1382,22 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>153679</v>
+        <v>153717</v>
       </c>
       <c r="F24" t="n">
-        <v>80669</v>
+        <v>80620</v>
       </c>
       <c r="G24" t="n">
-        <v>15431</v>
+        <v>15417</v>
       </c>
       <c r="H24" t="n">
-        <v>9165</v>
+        <v>9184</v>
       </c>
       <c r="I24" t="n">
-        <v>7715</v>
+        <v>7748</v>
       </c>
       <c r="J24" t="n">
-        <v>40699</v>
+        <v>40748</v>
       </c>
     </row>
     <row r="25">
@@ -1462,22 +1462,22 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2950</v>
+        <v>2954</v>
       </c>
       <c r="F26" t="n">
         <v>1448</v>
       </c>
       <c r="G26" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H26" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I26" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J26" t="n">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="27">
@@ -1571,19 +1571,19 @@
         <v>1538</v>
       </c>
       <c r="F29" t="n">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="G29" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H29" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I29" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J29" t="n">
-        <v>709</v>
+        <v>731</v>
       </c>
     </row>
     <row r="30">
@@ -1688,19 +1688,19 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="F32" t="n">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G32" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H32" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I32" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J32" t="n">
         <v>695</v>
@@ -1728,22 +1728,22 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>20528</v>
+        <v>20529</v>
       </c>
       <c r="F33" t="n">
-        <v>12688</v>
+        <v>12683</v>
       </c>
       <c r="G33" t="n">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="H33" t="n">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="I33" t="n">
         <v>616</v>
       </c>
       <c r="J33" t="n">
-        <v>2457</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="34">
@@ -1808,22 +1808,22 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="F35" t="n">
-        <v>1297</v>
+        <v>1302</v>
       </c>
       <c r="G35" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H35" t="n">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="I35" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J35" t="n">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="36">
@@ -1888,13 +1888,13 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="F37" t="n">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="G37" t="n">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H37" t="n">
         <v>25</v>

</xml_diff>